<commit_message>
results: old folder w/ previous sheets; final results with confidence interval calculation
</commit_message>
<xml_diff>
--- a/results/backup.xlsx
+++ b/results/backup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="medias" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="improvement" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="improvement%" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="final" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="final-new" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="46">
   <si>
     <t xml:space="preserve">PSNR (dB) – médias</t>
   </si>
@@ -160,6 +161,9 @@
   <si>
     <t xml:space="preserve">MSSIM Improvement (%) - sigma=10</t>
   </si>
+  <si>
+    <t xml:space="preserve">PSNR Improv ( dB ) - sigma=10</t>
+  </si>
 </sst>
 </file>
 
@@ -174,13 +178,12 @@
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="24">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -203,7 +206,6 @@
       <color rgb="FF81D41A"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -225,6 +227,13 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -286,13 +295,73 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
+      <sz val="9"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF1C1C1C"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -302,8 +371,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB2B2B2"/>
-        <bgColor rgb="FFAFD095"/>
+        <fgColor rgb="FF333333"/>
+        <bgColor rgb="FF1C1C1C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1C1C1C"/>
+        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
     <fill>
@@ -365,7 +440,7 @@
     </border>
   </borders>
   <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -388,379 +463,479 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="91">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+  <cellXfs count="116">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -779,7 +954,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF000000"/>
         <sz val="11"/>
@@ -793,7 +967,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF000000"/>
         <sz val="11"/>
@@ -807,7 +980,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="1"/>
         <color rgb="FF81D41A"/>
@@ -873,7 +1045,7 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF1C1C1C"/>
       <rgbColor rgb="FF8D281E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -890,11 +1062,11 @@
   </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="5" sqref="K19:K31 K35:K47 K51:K63 K67:K79 K83:K95 K3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.34"/>
@@ -919,7 +1091,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1132,7 +1304,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1370,11 +1542,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="5" sqref="K19:K31 K35:K47 K51:K63 K67:K79 K83:K95 F19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.23"/>
@@ -1398,7 +1570,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" s="20" customFormat="true" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="20" customFormat="true" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1642,7 +1814,7 @@
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
     </row>
-    <row r="14" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="21" t="s">
         <v>20</v>
       </c>
@@ -1680,7 +1852,7 @@
       <c r="M14" s="26"/>
       <c r="N14" s="26"/>
     </row>
-    <row r="15" s="29" customFormat="true" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="29" customFormat="true" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
         <v>21</v>
       </c>
@@ -2569,11 +2741,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J37" activeCellId="5" sqref="K19:K31 K35:K47 K51:K63 K67:K79 K83:K95 J37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="7.75"/>
@@ -2601,7 +2773,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -3039,7 +3211,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -3503,11 +3675,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="5" sqref="K19:K31 K35:K47 K51:K63 K67:K79 K83:K95 A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="7.75"/>
@@ -3535,7 +3707,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -3973,7 +4145,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -4434,8 +4606,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G67" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K83" activeCellId="4" sqref="K19:K31 K35:K47 K51:K63 K67:K79 K83:K95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4463,7 +4635,7 @@
       <c r="H1" s="60"/>
       <c r="I1" s="60"/>
     </row>
-    <row r="2" s="63" customFormat="true" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="63" customFormat="true" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="61" t="s">
         <v>24</v>
       </c>
@@ -6328,7 +6500,7 @@
       <c r="H49" s="60"/>
       <c r="I49" s="60"/>
     </row>
-    <row r="50" s="63" customFormat="true" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="63" customFormat="true" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="61" t="s">
         <v>24</v>
       </c>
@@ -8242,7 +8414,7 @@
     <mergeCell ref="A94:B94"/>
     <mergeCell ref="A95:B95"/>
   </mergeCells>
-  <conditionalFormatting sqref="A51:I62 A3:I14 A83:I94 A19:I30 A35:I46 A67:I78">
+  <conditionalFormatting sqref="A51:I62 A83:I94 A19:I30 A35:I46 A67:I78 A3:I14">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
@@ -8250,7 +8422,1609 @@
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:I14 C83:I94 C19:I30 C35:I46 C67:I78">
+  <conditionalFormatting sqref="C83:I94 C19:I30 C35:I46 C67:I78 B3:I14">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>#ref!=#ref!</formula>
+    </cfRule>
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>#ref!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ47"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="58" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="58" width="6.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="59" width="7.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="58" width="1.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="91" width="5.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="58" width="1.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="58" width="9.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="58" width="6.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="58" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="58" width="1.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="58" width="7.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="15" style="58" width="11.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="1016" style="58" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1017" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="I1" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="N1" s="91"/>
+    </row>
+    <row r="2" s="63" customFormat="true" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="58"/>
+      <c r="N2" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C3" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D3" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E3" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G3" s="93" t="n">
+        <f aca="false">MAX($C3:$F3)</f>
+        <v>27</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="22" t="n">
+        <f aca="false">C3-$B3</f>
+        <v>6</v>
+      </c>
+      <c r="K3" s="22" t="n">
+        <f aca="false">D3-$B3</f>
+        <v>7</v>
+      </c>
+      <c r="L3" s="22" t="n">
+        <f aca="false">E3-$B3</f>
+        <v>8</v>
+      </c>
+      <c r="N3" s="93" t="n">
+        <f aca="false">MAX($J3:$M3)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D4" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E4" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G4" s="94" t="n">
+        <f aca="false">MAX($C4:$F4)</f>
+        <v>27</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="22" t="n">
+        <f aca="false">C4-$B4</f>
+        <v>6</v>
+      </c>
+      <c r="K4" s="22" t="n">
+        <f aca="false">D4-$B4</f>
+        <v>7</v>
+      </c>
+      <c r="L4" s="22" t="n">
+        <f aca="false">E4-$B4</f>
+        <v>8</v>
+      </c>
+      <c r="N4" s="94" t="n">
+        <f aca="false">MAX($J4:$M4)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E5" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G5" s="93" t="n">
+        <f aca="false">MAX($C5:$F5)</f>
+        <v>27</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="22" t="n">
+        <f aca="false">C5-$B5</f>
+        <v>6</v>
+      </c>
+      <c r="K5" s="22" t="n">
+        <f aca="false">D5-$B5</f>
+        <v>7</v>
+      </c>
+      <c r="L5" s="22" t="n">
+        <f aca="false">E5-$B5</f>
+        <v>8</v>
+      </c>
+      <c r="N5" s="93" t="n">
+        <f aca="false">MAX($J5:$M5)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C6" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E6" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G6" s="94" t="n">
+        <f aca="false">MAX($C6:$F6)</f>
+        <v>27</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="22" t="n">
+        <f aca="false">C6-$B6</f>
+        <v>6</v>
+      </c>
+      <c r="K6" s="22" t="n">
+        <f aca="false">D6-$B6</f>
+        <v>7</v>
+      </c>
+      <c r="L6" s="22" t="n">
+        <f aca="false">E6-$B6</f>
+        <v>8</v>
+      </c>
+      <c r="N6" s="94" t="n">
+        <f aca="false">MAX($J6:$M6)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C7" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E7" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G7" s="93" t="n">
+        <f aca="false">MAX($C7:$F7)</f>
+        <v>27</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="22" t="n">
+        <f aca="false">C7-$B7</f>
+        <v>6</v>
+      </c>
+      <c r="K7" s="22" t="n">
+        <f aca="false">D7-$B7</f>
+        <v>7</v>
+      </c>
+      <c r="L7" s="22" t="n">
+        <f aca="false">E7-$B7</f>
+        <v>8</v>
+      </c>
+      <c r="N7" s="93" t="n">
+        <f aca="false">MAX($J7:$M7)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C8" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E8" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G8" s="94" t="n">
+        <f aca="false">MAX($C8:$F8)</f>
+        <v>27</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="22" t="n">
+        <f aca="false">C8-$B8</f>
+        <v>6</v>
+      </c>
+      <c r="K8" s="22" t="n">
+        <f aca="false">D8-$B8</f>
+        <v>7</v>
+      </c>
+      <c r="L8" s="22" t="n">
+        <f aca="false">E8-$B8</f>
+        <v>8</v>
+      </c>
+      <c r="N8" s="94" t="n">
+        <f aca="false">MAX($J8:$M8)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C9" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E9" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G9" s="93" t="n">
+        <f aca="false">MAX($C9:$F9)</f>
+        <v>27</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="22" t="n">
+        <f aca="false">C9-$B9</f>
+        <v>6</v>
+      </c>
+      <c r="K9" s="22" t="n">
+        <f aca="false">D9-$B9</f>
+        <v>7</v>
+      </c>
+      <c r="L9" s="22" t="n">
+        <f aca="false">E9-$B9</f>
+        <v>8</v>
+      </c>
+      <c r="N9" s="93" t="n">
+        <f aca="false">MAX($J9:$M9)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C10" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D10" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E10" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G10" s="94" t="n">
+        <f aca="false">MAX($C10:$F10)</f>
+        <v>27</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="22" t="n">
+        <f aca="false">C10-$B10</f>
+        <v>6</v>
+      </c>
+      <c r="K10" s="22" t="n">
+        <f aca="false">D10-$B10</f>
+        <v>7</v>
+      </c>
+      <c r="L10" s="22" t="n">
+        <f aca="false">E10-$B10</f>
+        <v>8</v>
+      </c>
+      <c r="N10" s="94" t="n">
+        <f aca="false">MAX($J10:$M10)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C11" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D11" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E11" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G11" s="93" t="n">
+        <f aca="false">MAX($C11:$F11)</f>
+        <v>27</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="22" t="n">
+        <f aca="false">C11-$B11</f>
+        <v>6</v>
+      </c>
+      <c r="K11" s="22" t="n">
+        <f aca="false">D11-$B11</f>
+        <v>7</v>
+      </c>
+      <c r="L11" s="22" t="n">
+        <f aca="false">E11-$B11</f>
+        <v>8</v>
+      </c>
+      <c r="N11" s="93" t="n">
+        <f aca="false">MAX($J11:$M11)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C12" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E12" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G12" s="94" t="n">
+        <f aca="false">MAX($C12:$F12)</f>
+        <v>27</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="22" t="n">
+        <f aca="false">C12-$B12</f>
+        <v>6</v>
+      </c>
+      <c r="K12" s="22" t="n">
+        <f aca="false">D12-$B12</f>
+        <v>7</v>
+      </c>
+      <c r="L12" s="22" t="n">
+        <f aca="false">E12-$B12</f>
+        <v>8</v>
+      </c>
+      <c r="N12" s="94" t="n">
+        <f aca="false">MAX($J12:$M12)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C13" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D13" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E13" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G13" s="93" t="n">
+        <f aca="false">MAX($C13:$F13)</f>
+        <v>27</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="22" t="n">
+        <f aca="false">C13-$B13</f>
+        <v>6</v>
+      </c>
+      <c r="K13" s="22" t="n">
+        <f aca="false">D13-$B13</f>
+        <v>7</v>
+      </c>
+      <c r="L13" s="22" t="n">
+        <f aca="false">E13-$B13</f>
+        <v>8</v>
+      </c>
+      <c r="N13" s="93" t="n">
+        <f aca="false">MAX($J13:$M13)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C14" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D14" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="E14" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G14" s="94" t="n">
+        <f aca="false">MAX($C14:$F14)</f>
+        <v>27</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="22" t="n">
+        <f aca="false">C14-$B14</f>
+        <v>6</v>
+      </c>
+      <c r="K14" s="22" t="n">
+        <f aca="false">D14-$B14</f>
+        <v>7</v>
+      </c>
+      <c r="L14" s="22" t="n">
+        <f aca="false">E14-$B14</f>
+        <v>8</v>
+      </c>
+      <c r="N14" s="94" t="n">
+        <f aca="false">MAX($J14:$M14)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" s="29" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="95" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="96" t="n">
+        <f aca="false">AVERAGE(B3:B14)</f>
+        <v>19</v>
+      </c>
+      <c r="C15" s="96" t="n">
+        <f aca="false">AVERAGE(C3:C14)</f>
+        <v>25</v>
+      </c>
+      <c r="D15" s="96" t="n">
+        <f aca="false">AVERAGE(D3:D14)</f>
+        <v>26</v>
+      </c>
+      <c r="E15" s="96" t="n">
+        <f aca="false">AVERAGE(E3:E14)</f>
+        <v>27</v>
+      </c>
+      <c r="F15" s="97"/>
+      <c r="G15" s="98" t="n">
+        <f aca="false">MAX($C15:$F15)</f>
+        <v>27</v>
+      </c>
+      <c r="H15" s="99"/>
+      <c r="I15" s="100" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="101" t="n">
+        <f aca="false">AVERAGE(J3:J14)</f>
+        <v>6</v>
+      </c>
+      <c r="K15" s="101" t="n">
+        <f aca="false">AVERAGE(K3:K14)</f>
+        <v>7</v>
+      </c>
+      <c r="L15" s="101" t="n">
+        <f aca="false">AVERAGE(L3:L14)</f>
+        <v>8</v>
+      </c>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98" t="n">
+        <f aca="false">MAX($J15:$M15)</f>
+        <v>8</v>
+      </c>
+      <c r="AMB15" s="58"/>
+      <c r="AMC15" s="0"/>
+      <c r="AMD15" s="0"/>
+      <c r="AME15" s="0"/>
+      <c r="AMF15" s="0"/>
+      <c r="AMG15" s="0"/>
+      <c r="AMH15" s="0"/>
+      <c r="AMI15" s="0"/>
+      <c r="AMJ15" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="30.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="I17" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="68"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+    </row>
+    <row r="18" s="63" customFormat="true" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="58"/>
+      <c r="N18" s="102" t="s">
+        <v>10</v>
+      </c>
+      <c r="AMC18" s="0"/>
+      <c r="AMD18" s="0"/>
+      <c r="AME18" s="0"/>
+      <c r="AMF18" s="0"/>
+      <c r="AMG18" s="0"/>
+      <c r="AMH18" s="0"/>
+      <c r="AMI18" s="0"/>
+      <c r="AMJ18" s="0"/>
+    </row>
+    <row r="19" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C19" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D19" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E19" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G19" s="103" t="n">
+        <f aca="false">MAX($C19:$F19)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I19" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="52" t="n">
+        <f aca="false">(C19-$B19)/$B19</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K19" s="52" t="n">
+        <f aca="false">(D19-$B19)/$B19</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L19" s="52" t="n">
+        <f aca="false">(E19-$B19)/$B19</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M19" s="85"/>
+      <c r="N19" s="104" t="n">
+        <f aca="false">MAX($J19:$M19)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC19" s="0"/>
+      <c r="AMD19" s="0"/>
+      <c r="AME19" s="0"/>
+      <c r="AMF19" s="0"/>
+      <c r="AMG19" s="0"/>
+      <c r="AMH19" s="0"/>
+      <c r="AMI19" s="0"/>
+      <c r="AMJ19" s="0"/>
+    </row>
+    <row r="20" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C20" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D20" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E20" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G20" s="105" t="n">
+        <f aca="false">MAX($C20:$F20)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I20" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="52" t="n">
+        <f aca="false">(C20-$B20)/$B20</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K20" s="52" t="n">
+        <f aca="false">(D20-$B20)/$B20</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L20" s="52" t="n">
+        <f aca="false">(E20-$B20)/$B20</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M20" s="85"/>
+      <c r="N20" s="106" t="n">
+        <f aca="false">MAX($J20:$M20)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC20" s="0"/>
+      <c r="AMD20" s="0"/>
+      <c r="AME20" s="0"/>
+      <c r="AMF20" s="0"/>
+      <c r="AMG20" s="0"/>
+      <c r="AMH20" s="0"/>
+      <c r="AMI20" s="0"/>
+      <c r="AMJ20" s="0"/>
+    </row>
+    <row r="21" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C21" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D21" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E21" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G21" s="103" t="n">
+        <f aca="false">MAX($C21:$F21)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I21" s="84" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="52" t="n">
+        <f aca="false">(C21-$B21)/$B21</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K21" s="52" t="n">
+        <f aca="false">(D21-$B21)/$B21</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L21" s="52" t="n">
+        <f aca="false">(E21-$B21)/$B21</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M21" s="85"/>
+      <c r="N21" s="104" t="n">
+        <f aca="false">MAX($J21:$M21)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC21" s="0"/>
+      <c r="AMD21" s="0"/>
+      <c r="AME21" s="0"/>
+      <c r="AMF21" s="0"/>
+      <c r="AMG21" s="0"/>
+      <c r="AMH21" s="0"/>
+      <c r="AMI21" s="0"/>
+      <c r="AMJ21" s="0"/>
+    </row>
+    <row r="22" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C22" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D22" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E22" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G22" s="105" t="n">
+        <f aca="false">MAX($C22:$F22)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I22" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="52" t="n">
+        <f aca="false">(C22-$B22)/$B22</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K22" s="52" t="n">
+        <f aca="false">(D22-$B22)/$B22</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L22" s="52" t="n">
+        <f aca="false">(E22-$B22)/$B22</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M22" s="85"/>
+      <c r="N22" s="106" t="n">
+        <f aca="false">MAX($J22:$M22)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC22" s="0"/>
+      <c r="AMD22" s="0"/>
+      <c r="AME22" s="0"/>
+      <c r="AMF22" s="0"/>
+      <c r="AMG22" s="0"/>
+      <c r="AMH22" s="0"/>
+      <c r="AMI22" s="0"/>
+      <c r="AMJ22" s="0"/>
+    </row>
+    <row r="23" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C23" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D23" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E23" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G23" s="103" t="n">
+        <f aca="false">MAX($C23:$F23)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I23" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="52" t="n">
+        <f aca="false">(C23-$B23)/$B23</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K23" s="52" t="n">
+        <f aca="false">(D23-$B23)/$B23</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L23" s="52" t="n">
+        <f aca="false">(E23-$B23)/$B23</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M23" s="85"/>
+      <c r="N23" s="104" t="n">
+        <f aca="false">MAX($J23:$M23)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC23" s="0"/>
+      <c r="AMD23" s="0"/>
+      <c r="AME23" s="0"/>
+      <c r="AMF23" s="0"/>
+      <c r="AMG23" s="0"/>
+      <c r="AMH23" s="0"/>
+      <c r="AMI23" s="0"/>
+      <c r="AMJ23" s="0"/>
+    </row>
+    <row r="24" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C24" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D24" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E24" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G24" s="105" t="n">
+        <f aca="false">MAX($C24:$F24)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I24" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" s="52" t="n">
+        <f aca="false">(C24-$B24)/$B24</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K24" s="52" t="n">
+        <f aca="false">(D24-$B24)/$B24</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L24" s="52" t="n">
+        <f aca="false">(E24-$B24)/$B24</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M24" s="85"/>
+      <c r="N24" s="106" t="n">
+        <f aca="false">MAX($J24:$M24)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC24" s="0"/>
+      <c r="AMD24" s="0"/>
+      <c r="AME24" s="0"/>
+      <c r="AMF24" s="0"/>
+      <c r="AMG24" s="0"/>
+      <c r="AMH24" s="0"/>
+      <c r="AMI24" s="0"/>
+      <c r="AMJ24" s="0"/>
+    </row>
+    <row r="25" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C25" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D25" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E25" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G25" s="103" t="n">
+        <f aca="false">MAX($C25:$F25)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I25" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" s="52" t="n">
+        <f aca="false">(C25-$B25)/$B25</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K25" s="52" t="n">
+        <f aca="false">(D25-$B25)/$B25</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L25" s="52" t="n">
+        <f aca="false">(E25-$B25)/$B25</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M25" s="85"/>
+      <c r="N25" s="104" t="n">
+        <f aca="false">MAX($J25:$M25)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC25" s="0"/>
+      <c r="AMD25" s="0"/>
+      <c r="AME25" s="0"/>
+      <c r="AMF25" s="0"/>
+      <c r="AMG25" s="0"/>
+      <c r="AMH25" s="0"/>
+      <c r="AMI25" s="0"/>
+      <c r="AMJ25" s="0"/>
+    </row>
+    <row r="26" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C26" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D26" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E26" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G26" s="105" t="n">
+        <f aca="false">MAX($C26:$F26)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I26" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="52" t="n">
+        <f aca="false">(C26-$B26)/$B26</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K26" s="52" t="n">
+        <f aca="false">(D26-$B26)/$B26</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L26" s="52" t="n">
+        <f aca="false">(E26-$B26)/$B26</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M26" s="85"/>
+      <c r="N26" s="106" t="n">
+        <f aca="false">MAX($J26:$M26)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC26" s="0"/>
+      <c r="AMD26" s="0"/>
+      <c r="AME26" s="0"/>
+      <c r="AMF26" s="0"/>
+      <c r="AMG26" s="0"/>
+      <c r="AMH26" s="0"/>
+      <c r="AMI26" s="0"/>
+      <c r="AMJ26" s="0"/>
+    </row>
+    <row r="27" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C27" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D27" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E27" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G27" s="103" t="n">
+        <f aca="false">MAX($C27:$F27)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I27" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="52" t="n">
+        <f aca="false">(C27-$B27)/$B27</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K27" s="52" t="n">
+        <f aca="false">(D27-$B27)/$B27</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L27" s="52" t="n">
+        <f aca="false">(E27-$B27)/$B27</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M27" s="85"/>
+      <c r="N27" s="104" t="n">
+        <f aca="false">MAX($J27:$M27)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC27" s="0"/>
+      <c r="AMD27" s="0"/>
+      <c r="AME27" s="0"/>
+      <c r="AMF27" s="0"/>
+      <c r="AMG27" s="0"/>
+      <c r="AMH27" s="0"/>
+      <c r="AMI27" s="0"/>
+      <c r="AMJ27" s="0"/>
+    </row>
+    <row r="28" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C28" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D28" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E28" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G28" s="105" t="n">
+        <f aca="false">MAX($C28:$F28)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I28" s="84" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" s="52" t="n">
+        <f aca="false">(C28-$B28)/$B28</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K28" s="52" t="n">
+        <f aca="false">(D28-$B28)/$B28</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L28" s="52" t="n">
+        <f aca="false">(E28-$B28)/$B28</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M28" s="85"/>
+      <c r="N28" s="106" t="n">
+        <f aca="false">MAX($J28:$M28)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC28" s="0"/>
+      <c r="AMD28" s="0"/>
+      <c r="AME28" s="0"/>
+      <c r="AMF28" s="0"/>
+      <c r="AMG28" s="0"/>
+      <c r="AMH28" s="0"/>
+      <c r="AMI28" s="0"/>
+      <c r="AMJ28" s="0"/>
+    </row>
+    <row r="29" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C29" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D29" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E29" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G29" s="103" t="n">
+        <f aca="false">MAX($C29:$F29)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I29" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="52" t="n">
+        <f aca="false">(C29-$B29)/$B29</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K29" s="52" t="n">
+        <f aca="false">(D29-$B29)/$B29</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L29" s="52" t="n">
+        <f aca="false">(E29-$B29)/$B29</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M29" s="85"/>
+      <c r="N29" s="104" t="n">
+        <f aca="false">MAX($J29:$M29)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC29" s="0"/>
+      <c r="AMD29" s="0"/>
+      <c r="AME29" s="0"/>
+      <c r="AMF29" s="0"/>
+      <c r="AMG29" s="0"/>
+      <c r="AMH29" s="0"/>
+      <c r="AMI29" s="0"/>
+      <c r="AMJ29" s="0"/>
+    </row>
+    <row r="30" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="36" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="C30" s="36" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="D30" s="36" t="n">
+        <v>1.998</v>
+      </c>
+      <c r="E30" s="36" t="n">
+        <v>2.998</v>
+      </c>
+      <c r="G30" s="105" t="n">
+        <f aca="false">MAX($C30:$F30)</f>
+        <v>2.998</v>
+      </c>
+      <c r="I30" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" s="52" t="n">
+        <f aca="false">(C30-$B30)/$B30</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K30" s="52" t="n">
+        <f aca="false">(D30-$B30)/$B30</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L30" s="52" t="n">
+        <f aca="false">(E30-$B30)/$B30</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M30" s="85"/>
+      <c r="N30" s="106" t="n">
+        <f aca="false">MAX($J30:$M30)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMC30" s="0"/>
+      <c r="AMD30" s="0"/>
+      <c r="AME30" s="0"/>
+      <c r="AMF30" s="0"/>
+      <c r="AMG30" s="0"/>
+      <c r="AMH30" s="0"/>
+      <c r="AMI30" s="0"/>
+      <c r="AMJ30" s="0"/>
+    </row>
+    <row r="31" s="44" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="108" t="n">
+        <f aca="false">AVERAGE(B19:B30)</f>
+        <v>0.987</v>
+      </c>
+      <c r="C31" s="108" t="n">
+        <f aca="false">AVERAGE(C19:C30)</f>
+        <v>0.998</v>
+      </c>
+      <c r="D31" s="108" t="n">
+        <f aca="false">AVERAGE(D19:D30)</f>
+        <v>1.998</v>
+      </c>
+      <c r="E31" s="108" t="n">
+        <f aca="false">AVERAGE(E19:E30)</f>
+        <v>2.998</v>
+      </c>
+      <c r="F31" s="109"/>
+      <c r="G31" s="110" t="n">
+        <f aca="false">MAX($C31:$F31)</f>
+        <v>2.998</v>
+      </c>
+      <c r="H31" s="111"/>
+      <c r="I31" s="112" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="113" t="n">
+        <f aca="false">AVERAGE(J19:J30)</f>
+        <v>0.011144883485309</v>
+      </c>
+      <c r="K31" s="113" t="n">
+        <f aca="false">AVERAGE(K19:K30)</f>
+        <v>1.02431610942249</v>
+      </c>
+      <c r="L31" s="113" t="n">
+        <f aca="false">AVERAGE(L19:L30)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="M31" s="114"/>
+      <c r="N31" s="115" t="n">
+        <f aca="false">MAX($J31:$M31)</f>
+        <v>2.03748733535968</v>
+      </c>
+      <c r="AMB31" s="76"/>
+      <c r="AMC31" s="0"/>
+      <c r="AMD31" s="0"/>
+      <c r="AME31" s="0"/>
+      <c r="AMF31" s="0"/>
+      <c r="AMG31" s="0"/>
+      <c r="AMH31" s="0"/>
+      <c r="AMI31" s="0"/>
+      <c r="AMJ31" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="I33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="23.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="58"/>
+      <c r="AMB34" s="0"/>
+    </row>
+    <row r="35" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="AMB35" s="0"/>
+      <c r="AMC35" s="0"/>
+      <c r="AMD35" s="0"/>
+      <c r="AME35" s="0"/>
+      <c r="AMF35" s="0"/>
+      <c r="AMG35" s="0"/>
+      <c r="AMH35" s="0"/>
+      <c r="AMI35" s="0"/>
+      <c r="AMJ35" s="0"/>
+    </row>
+    <row r="36" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="AMB36" s="0"/>
+      <c r="AMC36" s="0"/>
+      <c r="AMD36" s="0"/>
+      <c r="AME36" s="0"/>
+      <c r="AMF36" s="0"/>
+      <c r="AMG36" s="0"/>
+      <c r="AMH36" s="0"/>
+      <c r="AMI36" s="0"/>
+      <c r="AMJ36" s="0"/>
+    </row>
+    <row r="37" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="AMB37" s="0"/>
+      <c r="AMC37" s="0"/>
+      <c r="AMD37" s="0"/>
+      <c r="AME37" s="0"/>
+      <c r="AMF37" s="0"/>
+      <c r="AMG37" s="0"/>
+      <c r="AMH37" s="0"/>
+      <c r="AMI37" s="0"/>
+      <c r="AMJ37" s="0"/>
+    </row>
+    <row r="38" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="AMB38" s="0"/>
+      <c r="AMC38" s="0"/>
+      <c r="AMD38" s="0"/>
+      <c r="AME38" s="0"/>
+      <c r="AMF38" s="0"/>
+      <c r="AMG38" s="0"/>
+      <c r="AMH38" s="0"/>
+      <c r="AMI38" s="0"/>
+      <c r="AMJ38" s="0"/>
+    </row>
+    <row r="39" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="AMB39" s="0"/>
+      <c r="AMC39" s="0"/>
+      <c r="AMD39" s="0"/>
+      <c r="AME39" s="0"/>
+      <c r="AMF39" s="0"/>
+      <c r="AMG39" s="0"/>
+      <c r="AMH39" s="0"/>
+      <c r="AMI39" s="0"/>
+      <c r="AMJ39" s="0"/>
+    </row>
+    <row r="40" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="AMB40" s="0"/>
+      <c r="AMC40" s="0"/>
+      <c r="AMD40" s="0"/>
+      <c r="AME40" s="0"/>
+      <c r="AMF40" s="0"/>
+      <c r="AMG40" s="0"/>
+      <c r="AMH40" s="0"/>
+      <c r="AMI40" s="0"/>
+      <c r="AMJ40" s="0"/>
+    </row>
+    <row r="41" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="AMB41" s="0"/>
+      <c r="AMC41" s="0"/>
+      <c r="AMD41" s="0"/>
+      <c r="AME41" s="0"/>
+      <c r="AMF41" s="0"/>
+      <c r="AMG41" s="0"/>
+      <c r="AMH41" s="0"/>
+      <c r="AMI41" s="0"/>
+      <c r="AMJ41" s="0"/>
+    </row>
+    <row r="42" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="AMB42" s="0"/>
+      <c r="AMC42" s="0"/>
+      <c r="AMD42" s="0"/>
+      <c r="AME42" s="0"/>
+      <c r="AMF42" s="0"/>
+      <c r="AMG42" s="0"/>
+      <c r="AMH42" s="0"/>
+      <c r="AMI42" s="0"/>
+      <c r="AMJ42" s="0"/>
+    </row>
+    <row r="43" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="AMB43" s="0"/>
+      <c r="AMC43" s="0"/>
+      <c r="AMD43" s="0"/>
+      <c r="AME43" s="0"/>
+      <c r="AMF43" s="0"/>
+      <c r="AMG43" s="0"/>
+      <c r="AMH43" s="0"/>
+      <c r="AMI43" s="0"/>
+      <c r="AMJ43" s="0"/>
+    </row>
+    <row r="44" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="AMB44" s="0"/>
+      <c r="AMC44" s="0"/>
+      <c r="AMD44" s="0"/>
+      <c r="AME44" s="0"/>
+      <c r="AMF44" s="0"/>
+      <c r="AMG44" s="0"/>
+      <c r="AMH44" s="0"/>
+      <c r="AMI44" s="0"/>
+      <c r="AMJ44" s="0"/>
+    </row>
+    <row r="45" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
+      <c r="F45" s="0"/>
+      <c r="AMB45" s="0"/>
+      <c r="AMC45" s="0"/>
+      <c r="AMD45" s="0"/>
+      <c r="AME45" s="0"/>
+      <c r="AMF45" s="0"/>
+      <c r="AMG45" s="0"/>
+      <c r="AMH45" s="0"/>
+      <c r="AMI45" s="0"/>
+      <c r="AMJ45" s="0"/>
+    </row>
+    <row r="46" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0"/>
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
+      <c r="F46" s="0"/>
+      <c r="AMB46" s="0"/>
+      <c r="AMC46" s="0"/>
+      <c r="AMD46" s="0"/>
+      <c r="AME46" s="0"/>
+      <c r="AMF46" s="0"/>
+      <c r="AMG46" s="0"/>
+      <c r="AMH46" s="0"/>
+      <c r="AMI46" s="0"/>
+      <c r="AMJ46" s="0"/>
+    </row>
+    <row r="47" s="90" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0"/>
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
+      <c r="E47" s="0"/>
+      <c r="F47" s="0"/>
+      <c r="AMA47" s="85"/>
+      <c r="AMB47" s="0"/>
+      <c r="AMC47" s="0"/>
+      <c r="AMD47" s="0"/>
+      <c r="AME47" s="0"/>
+      <c r="AMF47" s="0"/>
+      <c r="AMG47" s="0"/>
+      <c r="AMH47" s="0"/>
+      <c r="AMI47" s="0"/>
+      <c r="AMJ47" s="0"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="I17:L17"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A3:E14 A19:E30 I3:L14 I19:L30">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>ISODD(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:E14 J3:L14 J19:L30">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>#ref!=#ref!</formula>
     </cfRule>

</xml_diff>